<commit_message>
fix slicing path fd2f71c9cb6aa934df1cd88faf30d32bb9c82555
</commit_message>
<xml_diff>
--- a/389-mapping---projet-personnalisé/ig/StructureDefinition-tddui-goal-objectif.xlsx
+++ b/389-mapping---projet-personnalisé/ig/StructureDefinition-tddui-goal-objectif.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-11-18T10:31:28+00:00</t>
+    <t>2025-11-18T14:30:08+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1111,7 +1111,7 @@
     <t>There's a need to capture information about the goal that doesn't actually describe the goal.</t>
   </si>
   <si>
-    <t xml:space="preserve">pattern:extension.where(url = 'http://hl7.org/fhir/StructureDefinition/goal-note-extension').valueCode}
+    <t xml:space="preserve">pattern:extension('https://interop.esante.gouv.fr/ig/fhir/tddui/StructureDefinition/tddui-goal-note').value}
 </t>
   </si>
   <si>
@@ -1734,7 +1734,7 @@
     <col min="25" max="25" width="131.83984375" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="56.23828125" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="5.44140625" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="81.8359375" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="83.765625" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="36.0390625" customWidth="true" bestFit="true"/>
     <col min="30" max="30" width="14.7578125" customWidth="true" bestFit="true"/>
     <col min="31" max="31" width="12.359375" customWidth="true" bestFit="true" hidden="true"/>

</xml_diff>